<commit_message>
Add About and FAQs as sites. Icons need work and better placement. #45.
</commit_message>
<xml_diff>
--- a/src/assets/media.xlsx
+++ b/src/assets/media.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Media" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="136">
   <si>
     <t>category</t>
   </si>
@@ -374,6 +374,72 @@
   </si>
   <si>
     <t>The rich aquatic life that inhabited river waters and shorelines would have supplied the community with food for sustenance and materials for tool and craft production. Mississippian pottery vessels often include likenesses, or effigies, that represent ducks, geese, and other waterfowl along with a variety of fish, reptiles, and amphibians. Although the precise meaning behind these effigies is unknown, riverine animals clearly played a significant role in the lives of the Mississippian people. </t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>Indiana-Map.jpg</t>
+  </si>
+  <si>
+    <t>Indiana Map</t>
+  </si>
+  <si>
+    <t>This map illustrates the location of  Angel Mounds Historic Site on the banks of the Ohio River in southwest Indiana.</t>
+  </si>
+  <si>
+    <t>MississippianSitesMap.jpg</t>
+  </si>
+  <si>
+    <t>Mississippian Sites</t>
+  </si>
+  <si>
+    <t>This map illustrates the locations of other Mississippian sites on the lower Ohio River and confluence area. </t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>about.tmpl.html</t>
+  </si>
+  <si>
+    <t>About Angel Mounds</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>FAQ</t>
+  </si>
+  <si>
+    <t>faq-1.tmpl.html</t>
+  </si>
+  <si>
+    <t>FAQ 1</t>
+  </si>
+  <si>
+    <t>faq-2.tmpl.html</t>
+  </si>
+  <si>
+    <t>FAQ 2</t>
+  </si>
+  <si>
+    <t>faq-3.tmpl.html</t>
+  </si>
+  <si>
+    <t>FAQ 3</t>
+  </si>
+  <si>
+    <t>faq-4.tmpl.html</t>
+  </si>
+  <si>
+    <t>FAQ 4</t>
+  </si>
+  <si>
+    <t>faq-5.tmpl.html</t>
+  </si>
+  <si>
+    <t>FAQ 5</t>
   </si>
   <si>
     <t>Mounds</t>
@@ -506,7 +572,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -533,18 +599,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -640,12 +694,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:31"/>
+  <dimension ref="1:39"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -657,7 +711,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.6632653061224"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8877551020408"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -736,13 +790,13 @@
       <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="6" t="n">
@@ -765,7 +819,7 @@
       <c r="C5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -814,7 +868,7 @@
       <c r="D7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>27</v>
       </c>
       <c r="F7" s="0" t="n">
@@ -831,13 +885,13 @@
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="7" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="6" t="n">
@@ -863,7 +917,7 @@
       <c r="D9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F9" s="0" t="n">
@@ -886,7 +940,7 @@
       <c r="D10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="0" t="n">
@@ -906,7 +960,7 @@
       <c r="D11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="0" t="n">
@@ -929,7 +983,7 @@
       <c r="D12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="8" t="s">
         <v>43</v>
       </c>
       <c r="F12" s="0" t="n">
@@ -949,10 +1003,10 @@
       <c r="C13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="5" t="s">
         <v>46</v>
       </c>
       <c r="F13" s="6" t="n">
@@ -975,10 +1029,10 @@
       <c r="C14" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="7" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="0" t="n">
@@ -998,7 +1052,7 @@
       <c r="C15" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1021,10 +1075,10 @@
       <c r="C16" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F16" s="0" t="n">
@@ -1044,7 +1098,7 @@
       <c r="C17" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>58</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -1067,7 +1121,7 @@
       <c r="C18" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="4" t="s">
         <v>61</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -1090,7 +1144,7 @@
       <c r="C19" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -1113,10 +1167,10 @@
       <c r="C20" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="7" t="s">
         <v>68</v>
       </c>
       <c r="F20" s="6" t="n">
@@ -1129,26 +1183,26 @@
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
-    <row r="21" s="12" customFormat="true" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="9" customFormat="true" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="12" t="n">
+      <c r="F21" s="9" t="n">
         <v>1920</v>
       </c>
-      <c r="G21" s="12" t="n">
+      <c r="G21" s="9" t="n">
         <v>1080</v>
       </c>
       <c r="AMH21" s="0"/>
@@ -1165,7 +1219,7 @@
       <c r="C22" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="4" t="s">
         <v>75</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -1283,7 +1337,7 @@
       <c r="D27" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="7" t="s">
         <v>92</v>
       </c>
       <c r="F27" s="0" t="n">
@@ -1306,7 +1360,7 @@
       <c r="D28" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="7" t="s">
         <v>95</v>
       </c>
       <c r="F28" s="0" t="n">
@@ -1329,7 +1383,7 @@
       <c r="D29" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F29" s="0" t="n">
@@ -1352,7 +1406,7 @@
       <c r="D30" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="7" t="s">
         <v>101</v>
       </c>
       <c r="F30" s="0" t="n">
@@ -1375,7 +1429,7 @@
       <c r="D31" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="7" t="s">
         <v>104</v>
       </c>
       <c r="F31" s="0" t="n">
@@ -1383,6 +1437,190 @@
       </c>
       <c r="G31" s="0" t="n">
         <v>1065</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>1028</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>3150</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -1445,47 +1683,47 @@
     </row>
     <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add layoutAngle property for line layout. Close #60.
</commit_message>
<xml_diff>
--- a/src/assets/media.xlsx
+++ b/src/assets/media.xlsx
@@ -388,6 +388,18 @@
     <t>This map illustrates the location of  Angel Mounds Historic Site on the banks of the Ohio River in southwest Indiana.</t>
   </si>
   <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>about.tmpl.html</t>
+  </si>
+  <si>
+    <t>About Angel Mounds</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
     <t>MississippianSitesMap.jpg</t>
   </si>
   <si>
@@ -395,18 +407,6 @@
   </si>
   <si>
     <t>This map illustrates the locations of other Mississippian sites on the lower Ohio River and confluence area. </t>
-  </si>
-  <si>
-    <t>html</t>
-  </si>
-  <si>
-    <t>about.tmpl.html</t>
-  </si>
-  <si>
-    <t>About Angel Mounds</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>FAQ</t>
@@ -694,12 +694,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:39"/>
+  <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1462,35 +1462,35 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>105</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>3150</v>
+        <v>1000</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>1962</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>105</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>112</v>
+        <v>8</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>113</v>
@@ -1502,10 +1502,10 @@
         <v>115</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>1000</v>
+        <v>3150</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>1000</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1513,7 +1513,7 @@
         <v>116</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>117</v>
@@ -1522,7 +1522,7 @@
         <v>118</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>1000</v>
@@ -1536,7 +1536,7 @@
         <v>116</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>119</v>
@@ -1545,7 +1545,7 @@
         <v>120</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>1000</v>
@@ -1559,7 +1559,7 @@
         <v>116</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>121</v>
@@ -1568,7 +1568,7 @@
         <v>122</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>1000</v>
@@ -1582,7 +1582,7 @@
         <v>116</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>123</v>
@@ -1591,7 +1591,7 @@
         <v>124</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>1000</v>
@@ -1605,7 +1605,7 @@
         <v>116</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>125</v>
@@ -1614,7 +1614,7 @@
         <v>126</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>1000</v>
@@ -1623,6 +1623,7 @@
         <v>500</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add category to missing photo. Fix #64.
</commit_message>
<xml_diff>
--- a/src/assets/media.xlsx
+++ b/src/assets/media.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Media" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="136">
   <si>
     <t>category</t>
   </si>
@@ -694,27 +694,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:65536"/>
+  <dimension ref="1:39"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="63.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.6479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.6632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.01020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.6377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.83163265306122"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.76020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -737,7 +736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
@@ -760,7 +759,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -783,7 +782,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="4" s="6" customFormat="true" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="6" customFormat="true" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>7</v>
       </c>
@@ -809,7 +808,7 @@
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>7</v>
       </c>
@@ -832,7 +831,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="364.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>7</v>
       </c>
@@ -855,7 +854,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="404.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>24</v>
       </c>
@@ -878,7 +877,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="8" s="6" customFormat="true" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="6" customFormat="true" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>24</v>
       </c>
@@ -904,7 +903,7 @@
       <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -927,7 +926,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="297" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>24</v>
       </c>
@@ -950,7 +949,10 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>24</v>
+      </c>
       <c r="B11" s="0" t="s">
         <v>8</v>
       </c>
@@ -970,7 +972,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="323.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>40</v>
       </c>
@@ -993,7 +995,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="13" s="6" customFormat="true" ht="377.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="6" customFormat="true" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>40</v>
       </c>
@@ -1019,7 +1021,7 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" customFormat="false" ht="364.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>40</v>
       </c>
@@ -1042,7 +1044,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="391" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>40</v>
       </c>
@@ -1065,7 +1067,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="364.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>40</v>
       </c>
@@ -1088,7 +1090,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>56</v>
       </c>
@@ -1111,7 +1113,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>56</v>
       </c>
@@ -1134,7 +1136,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="287.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>56</v>
       </c>
@@ -1157,7 +1159,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="20" s="6" customFormat="true" ht="431.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="6" customFormat="true" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>56</v>
       </c>
@@ -1183,7 +1185,7 @@
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
-    <row r="21" s="9" customFormat="true" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="9" customFormat="true" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>56</v>
       </c>
@@ -1209,7 +1211,7 @@
       <c r="AMI21" s="0"/>
       <c r="AMJ21" s="0"/>
     </row>
-    <row r="22" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>73</v>
       </c>
@@ -1232,7 +1234,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>73</v>
       </c>
@@ -1255,7 +1257,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="297" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>73</v>
       </c>
@@ -1278,7 +1280,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="323.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>73</v>
       </c>
@@ -1301,7 +1303,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>73</v>
       </c>
@@ -1324,7 +1326,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="377.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>89</v>
       </c>
@@ -1347,7 +1349,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>89</v>
       </c>
@@ -1370,7 +1372,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>89</v>
       </c>
@@ -1393,7 +1395,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>89</v>
       </c>
@@ -1416,7 +1418,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>89</v>
       </c>
@@ -1439,7 +1441,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>105</v>
       </c>
@@ -1462,7 +1464,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>105</v>
       </c>
@@ -1485,7 +1487,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>105</v>
       </c>
@@ -1508,7 +1510,7 @@
         <v>1962</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>116</v>
       </c>
@@ -1531,7 +1533,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>116</v>
       </c>
@@ -1554,7 +1556,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>116</v>
       </c>
@@ -1577,7 +1579,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>116</v>
       </c>
@@ -1600,7 +1602,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>116</v>
       </c>
@@ -1623,7 +1625,6 @@
         <v>500</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add FAQ/About iFrame template
</commit_message>
<xml_diff>
--- a/src/assets/media.xlsx
+++ b/src/assets/media.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Media" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,11 +15,16 @@
     <definedName function="false" hidden="false" name="Themes" vbProcedure="false">List!$A$1:$A$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="139">
   <si>
     <t>category</t>
   </si>
@@ -226,6 +231,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Stone axes and celts were useful for a range of tasks like chopping wood, clearing land, digging, and building houses. Archaeologists use the term </t>
     </r>
     <r>
@@ -249,23 +260,13 @@
     </r>
     <r>
       <rPr>
-        <i val="true"/>
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>celt</t>
+      <t>celt is used to refer to those without grooves. Celts are typically found at Mississippian sites like Angel, whereas grooved axes are more common during the earlier Archaic period. Both examples shown here were found during excavations in the East Village at Angel. The small grooved axe is made from quartzite.  It may have been collected from an earlier site by someone living at Angel, or it may have arrived at the site as a trade item. The celt is made from a type of chert native to Tennessee, also suggesting the trade of materials and tools among different regions.   </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> is used to refer to those without grooves. Celts are typically found at Mississippian sites like Angel, whereas grooved axes are more common during the earlier Archaic period. Both examples shown here were found during excavations in the East Village at Angel. The small grooved axe is made from quartzite.  It may have been collected from an earlier site by someone living at Angel, or it may have arrived at the site as a trade item. The celt is made from a type of chert native to Tennessee, also suggesting the trade of materials and tools among different regions.   </t>
-    </r>
   </si>
   <si>
     <t>video</t>
@@ -440,6 +441,15 @@
   </si>
   <si>
     <t>FAQ 5</t>
+  </si>
+  <si>
+    <t>iframe</t>
+  </si>
+  <si>
+    <t>assets/templates/faq/example5.html</t>
+  </si>
+  <si>
+    <t>FAQ </t>
   </si>
   <si>
     <t>Mounds</t>
@@ -476,7 +486,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -514,6 +524,13 @@
       <i val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -572,7 +589,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -609,12 +626,20 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -697,21 +722,21 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="bottomLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.6479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.6632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,7 +1195,7 @@
       <c r="D20" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="9" t="s">
         <v>68</v>
       </c>
       <c r="F20" s="6" t="n">
@@ -1183,26 +1208,26 @@
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
-    <row r="21" s="9" customFormat="true" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="10" customFormat="true" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="9" t="n">
+      <c r="F21" s="10" t="n">
         <v>1920</v>
       </c>
-      <c r="G21" s="9" t="n">
+      <c r="G21" s="10" t="n">
         <v>1080</v>
       </c>
       <c r="AMH21" s="0"/>
@@ -1620,6 +1645,29 @@
         <v>1000</v>
       </c>
       <c r="G39" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="G40" s="0" t="n">
         <v>500</v>
       </c>
     </row>
@@ -1648,8 +1696,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1684,47 +1732,47 @@
     </row>
     <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update content. Close #68.
</commit_message>
<xml_diff>
--- a/src/assets/media.xlsx
+++ b/src/assets/media.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Media" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,16 +15,11 @@
     <definedName function="false" hidden="false" name="Themes" vbProcedure="false">List!$A$1:$A$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="142">
   <si>
     <t>category</t>
   </si>
@@ -47,6 +42,9 @@
     <t>height</t>
   </si>
   <si>
+    <t>attribution</t>
+  </si>
+  <si>
     <t>Agriculture</t>
   </si>
   <si>
@@ -173,7 +171,7 @@
     <t>Pottery at Angel</t>
   </si>
   <si>
-    <t>Over a million of pieces of pottery have been collected from Angel during the course of archaeological excavations. The vast majority of those pieces are from plain vessels and would have been used for cooking, storage, serving, exchange, or transporting materials. The construction of these vessels likely took place in individual households. Occasionally, archaeologists find miniature versions of vessels. Their exact purposes are unknown, but it has been suggested that they could have been made by young people learning how to make vessels or they were used for storing small amounts of ritually significant materials (pigments, medicines, etc.).  </t>
+    <t>Over a million of pieces of pottery have been collected from Angel during the course of archaeological excavations. The vast majority of those pieces are from plain vessels and would have been used for cooking, storage, serving, exchange, or transporting materials. The construction of these vessels likely took place in individual households. Occasionally, archaeologists find miniature versions of vessels. Their exact purposes are unknown, but it has been suggested that they could have been made by young people learning how to make vessels or were used for storing small amounts of ritually significant materials (pigments, medicines, etc.).  </t>
   </si>
   <si>
     <t>Angel-stone-and-bone-tools.jpg</t>
@@ -182,7 +180,7 @@
     <t>Angel Tool Kit</t>
   </si>
   <si>
-    <t>Over a million pieces of stone and bone related to the manufacture of tools has been recovered from domestic contexts at Angel Mounds. Among the stone tools found at the site are celts (axes), projectile points, drills, engraving tools, hoes, and knives. Many of these tools were made from local stone material like Wyandotte chert, but others are made from materials that had to be transported from some distance away like Burlington (Missouri) and Dover (Tennessee) cherts. Bone tools found at the site include fish hooks, awls, needles, bone beamers (used for hide scraping). Fish hooks and beamers were typically made from deer bone, but finer tools like awls and needles were made from the hollow bones of birds.</t>
+    <t>Over a million pieces of stone and bone related to the manufacture of tools have been recovered from domestic contexts at Angel Mounds. Among the stone tools found at the site are celts (axes), projectile points, drills, engraving tools, hoes, and knives. Many of these tools were made from local stone material like Wyandotte chert, but others are made from materials that had to be transported from some distance away like Burlington (Missouri) and Dover (Tennessee) cherts. Bone tools found at the site include fish hooks, awls, needles, bone beamers (used for hide scraping). Fish hooks and beamers were typically made from deer bone, but finer tools like awls and needles were made from the hollow bones of birds.</t>
   </si>
   <si>
     <t>Chunkey-figure.jpg</t>
@@ -191,7 +189,7 @@
     <t>Chunkey Game</t>
   </si>
   <si>
-    <t>Chunkey was an important game that the people at Angel Mounds played. Chunkey was played by rolling a disc (made of stone or clay) across a flat surface, like a plaza, while players threw spears in an attempt to either make them land as close as possible to the stones final resting place or to hit the stone as it rolled. Depictions of chunkey players can be seen on shell gorgets and chunkey stones have been found at Angel. Chunkey is believed to have been developed before the Mississippian Period and then spread throughout the Midwest, Southeast, and Plains after A.D. 1050. The game was still played by the Creeks, Chickasaw, Choctaw, Muskogee, Cherokee, and Mandan after European contact.  </t>
+    <t>Chunkey was an important game that the people at Angel Mounds played. Chunkey was played by rolling a disc (made of stone or clay) across a flat surface, like a plaza, while players threw spears in an attempt to either make them land as close as possible to the stones final resting place or to hit the stone as it rolled. Depictions of chunkey players can be seen on shell gorgets (engraved pendants) and chunkey stones have been found at Angel. Chunkey is believed to have been developed before the Mississippian Period and then spread throughout the Midwest, Southeast, and Plains after A.D. 1050. The game was still played by the Creeks, Chickasaw, Choctaw, Muskogee, Cherokee, and Mandan after European contact.  </t>
   </si>
   <si>
     <t>Landscape</t>
@@ -231,12 +229,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t>Stone axes and celts were useful for a range of tasks like chopping wood, clearing land, digging, and building houses. Archaeologists use the term </t>
     </r>
     <r>
@@ -256,17 +248,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> to refer to those with a deep groove for attaching the stone to a handle, while the term </t>
+      <t> to refer to those with a deep groove for attaching the stone to a handle, while the term celt is used to refer to those without grooves. Celts are typically found at Mississippian sites like Angel, whereas grooved axes are more common during the earlier Archaic period. Both examples shown here were found during excavations in the East Village at Angel. The small grooved axe is made from quartzite.  It may have been collected from an earlier site by someone living at Angel, or it may have arrived at the site as a trade item. The celt is made from a type of chert native to Tennessee, also suggesting the trade of materials and tools among different regions.   </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>celt is used to refer to those without grooves. Celts are typically found at Mississippian sites like Angel, whereas grooved axes are more common during the earlier Archaic period. Both examples shown here were found during excavations in the East Village at Angel. The small grooved axe is made from quartzite.  It may have been collected from an earlier site by someone living at Angel, or it may have arrived at the site as a trade item. The celt is made from a type of chert native to Tennessee, also suggesting the trade of materials and tools among different regions.   </t>
-    </r>
   </si>
   <si>
     <t>video</t>
@@ -311,6 +294,9 @@
     <t>The exact reasons behind the increase in warfare are unknown, but researchers have suggested that climate change, resource uncertainty, environmental degradation, and political instability all played a role. Despite not knowing why warfare happened, we do know that warfare and warriors figured heavily in Mississippian religion and art before regional violence increased. Rock art, ceramic vessels, pipes, and copper objects (like the Rogan plate from Etowah, Georgia shown here) depict warriors and mythic persons holding weapons and severed heads.</t>
   </si>
   <si>
+    <t>Image Credit: Herb Roe (CC BY-SA 3.0), via Wikimedia</t>
+  </si>
+  <si>
     <t>1983FSPalisade-crop.jpg</t>
   </si>
   <si>
@@ -341,6 +327,9 @@
     <t>The Mississippian culture first developed along the Mississippi River and then expanded up through other major waterways like the Ohio River where the Angel site is located. The river served as a vital source of water for the large community and also provided food and material resources in the form of fish, shells, and other aquatic plants and animals. Periodic flooding along the river provided rich soil deposits for Mississippians to grow their crops. The river was also used for transportation to support an extensive trade network with other communities. Other important Mississippian sites located along the Ohio River include Kincaid Mounds in Illinois and Wycliffe Mounds in Kentucky. </t>
   </si>
   <si>
+    <t>Image credit: http://www.newburghmuseum.com/learn/newburgh-rivertown-trail/</t>
+  </si>
+  <si>
     <t>Mussel-Shells.jpg</t>
   </si>
   <si>
@@ -365,7 +354,7 @@
     <t>Fishing </t>
   </si>
   <si>
-    <t>Gar, Catfish, Buffalo fish, river pike, perch and bass are some of the types of fish that would have been available to people living at Angel. Fish hooks made from animal bone and fish bones have been recovered during Angel site excavations. Depending on the time of year, fish could have been harvested with nets, weirs, and bows-and-arrows, in addition to hook and line. It has been suggested that the presence of large riverine fish at upland Mississippian sites may indicate that fish were among the perishable goods that may have been traded for chert hoes, which were widely exchanged among Mississippian people.</t>
+    <t>Gar, catfish, buffalo fish, river pike, perch, and bass are some of the types of fish that would have been available to people living at Angel. Fish hooks made from animal bone and fish bones have been recovered during Angel site excavations. Depending on the time of year, fish could have been harvested with nets, weirs, and bows-and-arrows, in addition to hook and line. It has been suggested that the presence of large riverine fish at upland Mississippian sites may indicate that fish were among the perishable goods that may have been traded for chert hoes, which were widely exchanged among Mississippian people.</t>
   </si>
   <si>
     <t>Aquatic-Effigies.jpg</t>
@@ -589,7 +578,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -624,10 +613,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -722,9 +707,9 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
+      <selection pane="bottomLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -761,22 +746,25 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1000</v>
@@ -787,19 +775,19 @@
     </row>
     <row r="3" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1000</v>
@@ -810,19 +798,19 @@
     </row>
     <row r="4" s="6" customFormat="true" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>1000</v>
@@ -836,19 +824,19 @@
     </row>
     <row r="5" customFormat="false" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>1000</v>
@@ -859,19 +847,19 @@
     </row>
     <row r="6" customFormat="false" ht="364.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>1000</v>
@@ -882,19 +870,19 @@
     </row>
     <row r="7" customFormat="false" ht="404.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>1000</v>
@@ -905,19 +893,19 @@
     </row>
     <row r="8" s="6" customFormat="true" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F8" s="6" t="n">
         <v>1000</v>
@@ -931,19 +919,19 @@
     </row>
     <row r="9" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>1000</v>
@@ -954,19 +942,19 @@
     </row>
     <row r="10" customFormat="false" ht="297" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>1000</v>
@@ -976,17 +964,20 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="B11" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>1000</v>
@@ -997,19 +988,19 @@
     </row>
     <row r="12" customFormat="false" ht="323.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>1000</v>
@@ -1020,19 +1011,19 @@
     </row>
     <row r="13" s="6" customFormat="true" ht="377.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F13" s="6" t="n">
         <v>1000</v>
@@ -1046,19 +1037,19 @@
     </row>
     <row r="14" customFormat="false" ht="364.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>1000</v>
@@ -1069,19 +1060,19 @@
     </row>
     <row r="15" customFormat="false" ht="391" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>1000</v>
@@ -1090,21 +1081,21 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="364.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="404.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>1000</v>
@@ -1115,19 +1106,19 @@
     </row>
     <row r="17" customFormat="false" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>1000</v>
@@ -1138,19 +1129,19 @@
     </row>
     <row r="18" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>1000</v>
@@ -1161,19 +1152,19 @@
     </row>
     <row r="19" customFormat="false" ht="287.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>1000</v>
@@ -1184,19 +1175,19 @@
     </row>
     <row r="20" s="6" customFormat="true" ht="431.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="9" t="s">
         <v>68</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="F20" s="6" t="n">
         <v>1000</v>
@@ -1208,26 +1199,26 @@
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
-    <row r="21" s="10" customFormat="true" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="9" customFormat="true" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="D21" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="10" t="n">
+      <c r="E21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="9" t="n">
         <v>1920</v>
       </c>
-      <c r="G21" s="10" t="n">
+      <c r="G21" s="9" t="n">
         <v>1080</v>
       </c>
       <c r="AMH21" s="0"/>
@@ -1236,19 +1227,19 @@
     </row>
     <row r="22" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>1000</v>
@@ -1259,19 +1250,19 @@
     </row>
     <row r="23" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>1000</v>
@@ -1282,19 +1273,19 @@
     </row>
     <row r="24" customFormat="false" ht="297" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>1000</v>
@@ -1302,22 +1293,25 @@
       <c r="G24" s="0" t="n">
         <v>1313</v>
       </c>
+      <c r="H24" s="0" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="323.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>1000</v>
@@ -1328,19 +1322,19 @@
     </row>
     <row r="26" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>1000</v>
@@ -1351,19 +1345,19 @@
     </row>
     <row r="27" customFormat="false" ht="377.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>1000</v>
@@ -1371,22 +1365,25 @@
       <c r="G27" s="0" t="n">
         <v>1082</v>
       </c>
+      <c r="H27" s="0" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>1000</v>
@@ -1397,19 +1394,19 @@
     </row>
     <row r="29" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>1000</v>
@@ -1420,19 +1417,19 @@
     </row>
     <row r="30" customFormat="false" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>1000</v>
@@ -1443,19 +1440,19 @@
     </row>
     <row r="31" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>1000</v>
@@ -1466,19 +1463,19 @@
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>1028</v>
@@ -1489,19 +1486,19 @@
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>1000</v>
@@ -1512,19 +1509,19 @@
     </row>
     <row r="34" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>3150</v>
@@ -1535,19 +1532,19 @@
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>1000</v>
@@ -1558,19 +1555,19 @@
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>1000</v>
@@ -1581,19 +1578,19 @@
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>1000</v>
@@ -1604,19 +1601,19 @@
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>1000</v>
@@ -1627,19 +1624,19 @@
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>1000</v>
@@ -1650,19 +1647,19 @@
     </row>
     <row r="40" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>128</v>
+        <v>130</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>500</v>
@@ -1702,77 +1699,77 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Button Animate, layout changes
</commit_message>
<xml_diff>
--- a/src/assets/media.xlsx
+++ b/src/assets/media.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Media" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,11 +15,16 @@
     <definedName function="false" hidden="false" name="Themes" vbProcedure="false">List!$A$1:$A$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="117">
   <si>
     <t>category</t>
   </si>
@@ -229,11 +234,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Stone axes and celts were useful for a range of tasks like chopping wood, clearing land, digging, and building houses. Archaeologists use the term </t>
     </r>
     <r>
       <rPr>
-        <i val="true"/>
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -366,81 +377,6 @@
     <t>The rich aquatic life that inhabited river waters and shorelines would have supplied the community with food for sustenance and materials for tool and craft production. Mississippian pottery vessels often include likenesses, or effigies, that represent ducks, geese, and other waterfowl along with a variety of fish, reptiles, and amphibians. Although the precise meaning behind these effigies is unknown, riverine animals clearly played a significant role in the lives of the Mississippian people. </t>
   </si>
   <si>
-    <t>About</t>
-  </si>
-  <si>
-    <t>Indiana-Map.jpg</t>
-  </si>
-  <si>
-    <t>Indiana Map</t>
-  </si>
-  <si>
-    <t>This map illustrates the location of  Angel Mounds Historic Site on the banks of the Ohio River in southwest Indiana.</t>
-  </si>
-  <si>
-    <t>html</t>
-  </si>
-  <si>
-    <t>about.tmpl.html</t>
-  </si>
-  <si>
-    <t>About Angel Mounds</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>MississippianSitesMap.jpg</t>
-  </si>
-  <si>
-    <t>Mississippian Sites</t>
-  </si>
-  <si>
-    <t>This map illustrates the locations of other Mississippian sites on the lower Ohio River and confluence area. </t>
-  </si>
-  <si>
-    <t>FAQ</t>
-  </si>
-  <si>
-    <t>faq-1.tmpl.html</t>
-  </si>
-  <si>
-    <t>FAQ 1</t>
-  </si>
-  <si>
-    <t>faq-2.tmpl.html</t>
-  </si>
-  <si>
-    <t>FAQ 2</t>
-  </si>
-  <si>
-    <t>faq-3.tmpl.html</t>
-  </si>
-  <si>
-    <t>FAQ 3</t>
-  </si>
-  <si>
-    <t>faq-4.tmpl.html</t>
-  </si>
-  <si>
-    <t>FAQ 4</t>
-  </si>
-  <si>
-    <t>faq-5.tmpl.html</t>
-  </si>
-  <si>
-    <t>FAQ 5</t>
-  </si>
-  <si>
-    <t>iframe</t>
-  </si>
-  <si>
-    <t>assets/templates/faq/example5.html</t>
-  </si>
-  <si>
-    <t>FAQ </t>
-  </si>
-  <si>
     <t>Mounds</t>
   </si>
   <si>
@@ -475,7 +411,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -513,13 +449,6 @@
       <i val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -578,7 +507,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -621,10 +550,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -707,21 +632,21 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
+      <selection pane="bottomLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.5969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1461,213 +1386,15 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <v>1028</v>
-      </c>
-      <c r="G32" s="0" t="n">
-        <v>1382</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F33" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G33" s="0" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F34" s="0" t="n">
-        <v>3150</v>
-      </c>
-      <c r="G34" s="0" t="n">
-        <v>1962</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F35" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G35" s="0" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F36" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G36" s="0" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F37" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G37" s="0" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F38" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G38" s="0" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F39" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G39" s="0" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F40" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="G40" s="0" t="n">
-        <v>500</v>
-      </c>
-    </row>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1693,8 +1420,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1729,47 +1456,47 @@
     </row>
     <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add attribution to info pane. Misc styling. Close #70.
</commit_message>
<xml_diff>
--- a/src/assets/media.xlsx
+++ b/src/assets/media.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Media" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,11 +15,6 @@
     <definedName function="false" hidden="false" name="Themes" vbProcedure="false">List!$A$1:$A$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -234,13 +229,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t>Stone axes and celts were useful for a range of tasks like chopping wood, clearing land, digging, and building houses. Archaeologists use the term </t>
     </r>
     <r>
@@ -250,16 +238,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>axe</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> to refer to those with a deep groove for attaching the stone to a handle, while the term celt is used to refer to those without grooves. Celts are typically found at Mississippian sites like Angel, whereas grooved axes are more common during the earlier Archaic period. Both examples shown here were found during excavations in the East Village at Angel. The small grooved axe is made from quartzite.  It may have been collected from an earlier site by someone living at Angel, or it may have arrived at the site as a trade item. The celt is made from a type of chert native to Tennessee, also suggesting the trade of materials and tools among different regions.   </t>
+      <t>axe to refer to those with a deep groove for attaching the stone to a handle, while the term celt is used to refer to those without grooves. Celts are typically found at Mississippian sites like Angel, whereas grooved axes are more common during the earlier Archaic period. Both examples shown here were found during excavations in the East Village at Angel. The small grooved axe is made from quartzite.  It may have been collected from an earlier site by someone living at Angel, or it may have arrived at the site as a trade item. The celt is made from a type of chert native to Tennessee, also suggesting the trade of materials and tools among different regions.   </t>
     </r>
   </si>
   <si>
@@ -507,7 +486,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -542,6 +521,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -632,9 +615,9 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
+      <selection pane="bottomLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1111,7 +1094,7 @@
       <c r="D20" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="9" t="s">
         <v>69</v>
       </c>
       <c r="F20" s="6" t="n">
@@ -1124,26 +1107,26 @@
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
-    <row r="21" s="9" customFormat="true" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="10" customFormat="true" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="9" t="n">
+      <c r="F21" s="10" t="n">
         <v>1920</v>
       </c>
-      <c r="G21" s="9" t="n">
+      <c r="G21" s="10" t="n">
         <v>1080</v>
       </c>
       <c r="AMH21" s="0"/>

</xml_diff>

<commit_message>
Fix some image sizes. Sidesteps #71.
</commit_message>
<xml_diff>
--- a/src/assets/media.xlsx
+++ b/src/assets/media.xlsx
@@ -615,9 +615,9 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -750,7 +750,7 @@
         <v>1000</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>1046</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="364.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,7 +937,7 @@
         <v>1000</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>1049</v>
+        <v>1039</v>
       </c>
       <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
@@ -1196,7 +1196,7 @@
         <v>83</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>1313</v>
@@ -1297,7 +1297,7 @@
         <v>1000</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>1072</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1343,7 +1343,7 @@
         <v>1000</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>1243</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>